<commit_message>
add code sql uodate excell
</commit_message>
<xml_diff>
--- a/Android-code.xlsx
+++ b/Android-code.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hassan\Desktop\project_hassan\Shoping-\Shoping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hassan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EECEC5-B138-4AA6-A635-5A4C7A442B75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756AADCF-AA3F-482F-9BF4-07A5EE95B809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kotlin" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>project lib</t>
   </si>
@@ -174,6 +174,68 @@
     <t>میتونیم برای onclick از این PopupMenu.OnMenuItemClickListener
 اینترفیس استفاده کنیم</t>
   </si>
+  <si>
+    <t>webView.settings.javaScriptEnabled = true
+        webView.settings.builtInZoomControls = true
+        webView.settings.textZoom = 100
+        webView.webViewClient = WebViewClient()
+        webView.loadUrl(url)</t>
+  </si>
+  <si>
+    <t>Web View</t>
+  </si>
+  <si>
+    <t>if (intent.resolveActivity(context.packageManager) != null)
+                        context.startActivity(intent)</t>
+  </si>
+  <si>
+    <t>اگر اکتیویتیش وجود نداشته باشه استارتش نمیکنه
+از try/cach هم میتونیم استفاده کنیم</t>
+  </si>
+  <si>
+    <t>val view = LayoutInflater.from(context).inflate(R.layout.dialog_call_me, null)
+                AlertDialog.Builder(context)
+                    .setView(view)
+                    .show()</t>
+  </si>
+  <si>
+    <t>AlertDialog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    &lt;androidx.appcompat.widget.AppCompatEditText
+        android:id="@+id/edt_text_dialog_failure_report"
+        android:layout_width="0dp"
+        android:layout_height="wrap_content"
+        android:ems="10"
+        android:gravity="top"
+        android:hint="@string/text"
+        android:inputType="textMultiLine"
+        android:lines="3"
+        android:maxLines="10"
+        android:scrollbars="vertical"/&gt;
+        </t>
+  </si>
+  <si>
+    <t>تکست چند خطی</t>
+  </si>
+  <si>
+    <t>&lt;style name="DialogTheme" parent="Theme.AppCompat.Light.Dialog.Alert"&gt;
+        &lt;item name="buttonBarNegativeButtonStyle"&gt;@style/NegativeButton&lt;/item&gt;
+        &lt;item name="buttonBarPositiveButtonStyle"&gt;@style/PositiveButton&lt;/item&gt;
+    &lt;/style&gt;
+ &lt;style name="PositiveButton" parent="Widget.AppCompat.Button.ButtonBar.AlertDialog"&gt;
+        &lt;item name="android:textColor"&gt;@color/colorBlack&lt;/item&gt;
+        &lt;item name="android:textSize"&gt;16sp&lt;/item&gt;
+    &lt;/style&gt;
+&lt;style name="NegativeButton" parent="Widget.AppCompat.Button.ButtonBar.AlertDialog"&gt;
+        &lt;item name="android:textColor"&gt;@color/colorBlack&lt;/item&gt;
+        &lt;item name="android:textSize"&gt;16sp&lt;/item&gt;
+    &lt;/style&gt;</t>
+  </si>
+  <si>
+    <t>برای رنگ به متن Alert Dilog</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -236,6 +298,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,9 +582,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +598,7 @@
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -541,7 +606,7 @@
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -559,6 +624,30 @@
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -569,10 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA2AF12-07F6-4588-AB61-35C600F00118}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +701,22 @@
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add PROCEDURE :)))) 1400/02/05
</commit_message>
<xml_diff>
--- a/Android-code.xlsx
+++ b/Android-code.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hassan\Desktop\project_hassan\Shoping\Shoping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_bagheri\Desktop\android\app-shoping-hassan\project\AppShoping-master\AppShoping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E21DD-8DEC-406E-BBC2-5768165C4EE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Kotlin" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>project lib</t>
   </si>
@@ -265,11 +264,26 @@
             android:name=".activity.LoginActivity"
             android:theme="@style/fullScreen"/&gt;</t>
   </si>
+  <si>
+    <t>DROP PROCEDURE IF EXISTS `check_login`;
+CREATE PROCEDURE `check_login`(IN email VARCHAR(200) , IN pass VARCHAR(200))
+BEGIN
+  SELECT * FROM users
+  WHERE users.email COLLATE utf8_unicode_ci = email
+ AND
+ users.password COLLATE utf8_unicode_ci = pass
+ ;
+END;
+CALL check_login('hassan1@gmail.com','123456')</t>
+  </si>
+  <si>
+    <t>PROCEDURE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -610,7 +624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -694,10 +708,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -775,7 +789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -787,7 +801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -799,7 +813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -838,7 +852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -850,21 +864,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="75.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>